<commit_message>
Add lexicon search functionality to enhance query handling
</commit_message>
<xml_diff>
--- a/Capstone Dataset without Answers.xlsx
+++ b/Capstone Dataset without Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2fec667f7c86ea8/Important/Capstone/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="789" documentId="8_{BF4269A5-6DD2-4A5F-8985-34CC16678376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0C6B1A5-9E68-4642-9A2C-A98FBE99F774}"/>
+  <xr:revisionPtr revIDLastSave="790" documentId="8_{BF4269A5-6DD2-4A5F-8985-34CC16678376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73AA989F-9F45-461D-BFA2-C88DA30773BF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="20" activeTab="22" xr2:uid="{C4378324-5452-4919-A683-490F04C84E34}"/>
   </bookViews>
@@ -6117,7 +6117,7 @@
   <autoFilter ref="A1:G221" xr:uid="{7BB44F78-57CB-4377-BAEA-8EEA5DBEB624}">
     <filterColumn colId="0">
       <filters>
-        <filter val="B.9 Domain: Data protection and privacy"/>
+        <filter val="B.5 Domain: Compliance"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8295,7 +8295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C5A07-AF1D-4E42-9C62-6AFF1F9D3503}">
   <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
       <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
@@ -9038,7 +9038,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="25"/>
     </row>
-    <row r="40" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>276</v>
       </c>
@@ -9057,7 +9057,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="25"/>
     </row>
-    <row r="41" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>276</v>
       </c>
@@ -9076,7 +9076,7 @@
       <c r="F41" s="18"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>276</v>
       </c>
@@ -9095,7 +9095,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="25"/>
     </row>
-    <row r="43" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>276</v>
       </c>
@@ -9114,7 +9114,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="25"/>
     </row>
-    <row r="44" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>276</v>
       </c>
@@ -9133,7 +9133,7 @@
       <c r="F44" s="18"/>
       <c r="G44" s="26"/>
     </row>
-    <row r="45" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>276</v>
       </c>
@@ -9152,7 +9152,7 @@
       <c r="F45" s="18"/>
       <c r="G45" s="26"/>
     </row>
-    <row r="46" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>276</v>
       </c>
@@ -9171,7 +9171,7 @@
       <c r="F46" s="9"/>
       <c r="G46" s="25"/>
     </row>
-    <row r="47" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>276</v>
       </c>
@@ -9190,7 +9190,7 @@
       <c r="F47" s="9"/>
       <c r="G47" s="25"/>
     </row>
-    <row r="48" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>276</v>
       </c>
@@ -9754,7 +9754,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="25"/>
     </row>
-    <row r="78" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>383</v>
       </c>
@@ -9773,7 +9773,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="25"/>
     </row>
-    <row r="79" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>383</v>
       </c>
@@ -9792,7 +9792,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="25"/>
     </row>
-    <row r="80" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>383</v>
       </c>
@@ -9811,7 +9811,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="25"/>
     </row>
-    <row r="81" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>383</v>
       </c>
@@ -9830,7 +9830,7 @@
       <c r="F81" s="18"/>
       <c r="G81" s="26"/>
     </row>
-    <row r="82" spans="1:7" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="151.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>383</v>
       </c>
@@ -9849,7 +9849,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="25"/>
     </row>
-    <row r="83" spans="1:7" ht="151.80000000000001" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="151.80000000000001" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>383</v>
       </c>
@@ -9868,7 +9868,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="25"/>
     </row>
-    <row r="84" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="138" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>383</v>
       </c>
@@ -9887,7 +9887,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="25"/>
     </row>
-    <row r="85" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>383</v>
       </c>
@@ -9906,7 +9906,7 @@
       <c r="F85" s="18"/>
       <c r="G85" s="26"/>
     </row>
-    <row r="86" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>383</v>
       </c>
@@ -9925,7 +9925,7 @@
       <c r="F86" s="18"/>
       <c r="G86" s="26"/>
     </row>
-    <row r="87" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>383</v>
       </c>
@@ -9944,7 +9944,7 @@
       <c r="F87" s="18"/>
       <c r="G87" s="26"/>
     </row>
-    <row r="88" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>383</v>
       </c>
@@ -9963,7 +9963,7 @@
       <c r="F88" s="9"/>
       <c r="G88" s="25"/>
     </row>
-    <row r="89" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
         <v>383</v>
       </c>
@@ -9982,7 +9982,7 @@
       <c r="F89" s="9"/>
       <c r="G89" s="25"/>
     </row>
-    <row r="90" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>383</v>
       </c>
@@ -13059,14 +13059,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003C6AD2958B7004BABBF2542FA0759A5" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="82fe485139ae45ef5696bc26fc72e966">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4b56964bfa007738a55a3983173e6d0" ns3:_="">
     <xsd:import namespace="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
@@ -13248,6 +13240,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3907F4E3-FAD5-4253-8C8E-B07BB65EB7F4}">
   <ds:schemaRefs>
@@ -13257,16 +13257,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCDF0B-D2BA-4C39-8FF7-B71DDC9797CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0AACCDC-ECF2-4D5E-86C9-1CAB48FC3D42}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13282,4 +13272,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCDF0B-D2BA-4C39-8FF7-B71DDC9797CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Capstone Dataset without Answers.xlsx to .gitignore
</commit_message>
<xml_diff>
--- a/Capstone Dataset without Answers.xlsx
+++ b/Capstone Dataset without Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2fec667f7c86ea8/Important/Capstone/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="790" documentId="8_{BF4269A5-6DD2-4A5F-8985-34CC16678376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73AA989F-9F45-461D-BFA2-C88DA30773BF}"/>
+  <xr:revisionPtr revIDLastSave="791" documentId="8_{BF4269A5-6DD2-4A5F-8985-34CC16678376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F1E98B4-30D9-4186-BD27-656E364D296B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="20" activeTab="22" xr2:uid="{C4378324-5452-4919-A683-490F04C84E34}"/>
   </bookViews>
@@ -6117,7 +6117,7 @@
   <autoFilter ref="A1:G221" xr:uid="{7BB44F78-57CB-4377-BAEA-8EEA5DBEB624}">
     <filterColumn colId="0">
       <filters>
-        <filter val="B.5 Domain: Compliance"/>
+        <filter val="B.6 Domain: Audit"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8295,8 +8295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C5A07-AF1D-4E42-9C62-6AFF1F9D3503}">
   <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9038,7 +9038,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="25"/>
     </row>
-    <row r="40" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>276</v>
       </c>
@@ -9057,7 +9057,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="25"/>
     </row>
-    <row r="41" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>276</v>
       </c>
@@ -9076,7 +9076,7 @@
       <c r="F41" s="18"/>
       <c r="G41" s="26"/>
     </row>
-    <row r="42" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>276</v>
       </c>
@@ -9095,7 +9095,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="25"/>
     </row>
-    <row r="43" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>276</v>
       </c>
@@ -9114,7 +9114,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="25"/>
     </row>
-    <row r="44" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>276</v>
       </c>
@@ -9133,7 +9133,7 @@
       <c r="F44" s="18"/>
       <c r="G44" s="26"/>
     </row>
-    <row r="45" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>276</v>
       </c>
@@ -9152,7 +9152,7 @@
       <c r="F45" s="18"/>
       <c r="G45" s="26"/>
     </row>
-    <row r="46" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>276</v>
       </c>
@@ -9171,7 +9171,7 @@
       <c r="F46" s="9"/>
       <c r="G46" s="25"/>
     </row>
-    <row r="47" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>276</v>
       </c>
@@ -9190,7 +9190,7 @@
       <c r="F47" s="9"/>
       <c r="G47" s="25"/>
     </row>
-    <row r="48" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>276</v>
       </c>
@@ -9209,7 +9209,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="25"/>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>302</v>
       </c>
@@ -9226,7 +9226,7 @@
       <c r="F49" s="14"/>
       <c r="G49" s="24"/>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>302</v>
       </c>
@@ -9243,7 +9243,7 @@
       <c r="F50" s="14"/>
       <c r="G50" s="24"/>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>302</v>
       </c>
@@ -9260,7 +9260,7 @@
       <c r="F51" s="14"/>
       <c r="G51" s="24"/>
     </row>
-    <row r="52" spans="1:7" ht="138" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>302</v>
       </c>
@@ -9279,7 +9279,7 @@
       <c r="F52" s="18"/>
       <c r="G52" s="26"/>
     </row>
-    <row r="53" spans="1:7" ht="69" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="69" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>302</v>
       </c>
@@ -9298,7 +9298,7 @@
       <c r="F53" s="18"/>
       <c r="G53" s="26"/>
     </row>
-    <row r="54" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>302</v>
       </c>
@@ -9317,7 +9317,7 @@
       <c r="F54" s="18"/>
       <c r="G54" s="26"/>
     </row>
-    <row r="55" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>302</v>
       </c>
@@ -9336,7 +9336,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="25"/>
     </row>
-    <row r="56" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>302</v>
       </c>
@@ -13059,6 +13059,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003C6AD2958B7004BABBF2542FA0759A5" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="82fe485139ae45ef5696bc26fc72e966">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4b56964bfa007738a55a3983173e6d0" ns3:_="">
     <xsd:import namespace="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
@@ -13240,14 +13248,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3907F4E3-FAD5-4253-8C8E-B07BB65EB7F4}">
   <ds:schemaRefs>
@@ -13257,6 +13257,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCDF0B-D2BA-4C39-8FF7-B71DDC9797CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0AACCDC-ECF2-4D5E-86C9-1CAB48FC3D42}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13272,14 +13282,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCDF0B-D2BA-4C39-8FF7-B71DDC9797CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add grading scripts and evaluation logic; update Excel files
</commit_message>
<xml_diff>
--- a/Capstone Dataset without Answers.xlsx
+++ b/Capstone Dataset without Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2fec667f7c86ea8/Important/Capstone/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="796" documentId="8_{BF4269A5-6DD2-4A5F-8985-34CC16678376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFA29828-8427-46AC-B7B8-6277AC029C2B}"/>
+  <xr:revisionPtr revIDLastSave="799" documentId="8_{BF4269A5-6DD2-4A5F-8985-34CC16678376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19E1F90F-4EA7-4B44-BC7A-569E017E5283}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="20" activeTab="22" xr2:uid="{C4378324-5452-4919-A683-490F04C84E34}"/>
   </bookViews>
@@ -5923,6 +5923,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A5EDD2ED-F317-41E0-B9EA-6F42F9BE3CD9}" name="Table9" displayName="Table9" ref="A1:C10" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{A5EDD2ED-F317-41E0-B9EA-6F42F9BE3CD9}"/>
@@ -6113,7 +6117,7 @@
   <autoFilter ref="A1:G221" xr:uid="{7BB44F78-57CB-4377-BAEA-8EEA5DBEB624}">
     <filterColumn colId="0">
       <filters>
-        <filter val="B.22 Domain: Business continuity/Disaster recovery"/>
+        <filter val="B.18 Domain: Vulnerability assessment"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8291,8 +8295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C5A07-AF1D-4E42-9C62-6AFF1F9D3503}">
   <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="E194" sqref="E194:E203"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179:E180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11470,7 +11474,7 @@
       <c r="F169" s="9"/>
       <c r="G169" s="25"/>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>636</v>
       </c>
@@ -11487,7 +11491,7 @@
       <c r="F170" s="14"/>
       <c r="G170" s="24"/>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>636</v>
       </c>
@@ -11504,7 +11508,7 @@
       <c r="F171" s="14"/>
       <c r="G171" s="24"/>
     </row>
-    <row r="172" spans="1:7" ht="69" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" ht="69" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
         <v>636</v>
       </c>
@@ -11523,7 +11527,7 @@
       <c r="F172" s="9"/>
       <c r="G172" s="25"/>
     </row>
-    <row r="173" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
         <v>636</v>
       </c>
@@ -11542,7 +11546,7 @@
       <c r="F173" s="9"/>
       <c r="G173" s="25"/>
     </row>
-    <row r="174" spans="1:7" ht="69" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" ht="69" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
         <v>636</v>
       </c>
@@ -11561,7 +11565,7 @@
       <c r="F174" s="18"/>
       <c r="G174" s="26"/>
     </row>
-    <row r="175" spans="1:7" ht="138" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" ht="138" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
         <v>636</v>
       </c>
@@ -11580,7 +11584,7 @@
       <c r="F175" s="18"/>
       <c r="G175" s="26"/>
     </row>
-    <row r="176" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
         <v>636</v>
       </c>
@@ -11599,7 +11603,7 @@
       <c r="F176" s="18"/>
       <c r="G176" s="26"/>
     </row>
-    <row r="177" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
         <v>636</v>
       </c>
@@ -11618,7 +11622,7 @@
       <c r="F177" s="9"/>
       <c r="G177" s="25"/>
     </row>
-    <row r="178" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>636</v>
       </c>
@@ -11637,7 +11641,7 @@
       <c r="F178" s="9"/>
       <c r="G178" s="25"/>
     </row>
-    <row r="179" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>636</v>
       </c>
@@ -11656,7 +11660,7 @@
       <c r="F179" s="9"/>
       <c r="G179" s="25"/>
     </row>
-    <row r="180" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
         <v>636</v>
       </c>
@@ -12260,7 +12264,7 @@
       <c r="F211" s="9"/>
       <c r="G211" s="25"/>
     </row>
-    <row r="212" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
         <v>760</v>
       </c>
@@ -12277,7 +12281,7 @@
       <c r="F212" s="14"/>
       <c r="G212" s="24"/>
     </row>
-    <row r="213" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>760</v>
       </c>
@@ -12296,7 +12300,7 @@
       <c r="F213" s="18"/>
       <c r="G213" s="26"/>
     </row>
-    <row r="214" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
         <v>760</v>
       </c>
@@ -12315,7 +12319,7 @@
       <c r="F214" s="9"/>
       <c r="G214" s="25"/>
     </row>
-    <row r="215" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" ht="69" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
         <v>760</v>
       </c>
@@ -12334,7 +12338,7 @@
       <c r="F215" s="9"/>
       <c r="G215" s="25"/>
     </row>
-    <row r="216" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" ht="124.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
         <v>760</v>
       </c>
@@ -12353,7 +12357,7 @@
       <c r="F216" s="18"/>
       <c r="G216" s="26"/>
     </row>
-    <row r="217" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="7" t="s">
         <v>760</v>
       </c>
@@ -12372,7 +12376,7 @@
       <c r="F217" s="18"/>
       <c r="G217" s="26"/>
     </row>
-    <row r="218" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" ht="82.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="7" t="s">
         <v>760</v>
       </c>
@@ -12391,7 +12395,7 @@
       <c r="F218" s="18"/>
       <c r="G218" s="26"/>
     </row>
-    <row r="219" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" ht="110.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="7" t="s">
         <v>760</v>
       </c>
@@ -12410,7 +12414,7 @@
       <c r="F219" s="18"/>
       <c r="G219" s="26"/>
     </row>
-    <row r="220" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
         <v>760</v>
       </c>
@@ -12429,7 +12433,7 @@
       <c r="F220" s="9"/>
       <c r="G220" s="25"/>
     </row>
-    <row r="221" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" ht="96.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
         <v>760</v>
       </c>
@@ -13046,15 +13050,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003C6AD2958B7004BABBF2542FA0759A5" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="82fe485139ae45ef5696bc26fc72e966">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ba8e16aa-8cbb-4107-a8f6-a7403072b12e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4b56964bfa007738a55a3983173e6d0" ns3:_="">
     <xsd:import namespace="ba8e16aa-8cbb-4107-a8f6-a7403072b12e"/>
@@ -13236,6 +13231,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -13245,14 +13249,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3907F4E3-FAD5-4253-8C8E-B07BB65EB7F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0AACCDC-ECF2-4D5E-86C9-1CAB48FC3D42}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13270,6 +13266,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3907F4E3-FAD5-4253-8C8E-B07BB65EB7F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FBCDF0B-D2BA-4C39-8FF7-B71DDC9797CA}">
   <ds:schemaRefs>

</xml_diff>